<commit_message>
Add test scenario for booking
</commit_message>
<xml_diff>
--- a/data/restful_booker_test_scenarios.xlsx
+++ b/data/restful_booker_test_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\restful-booker-test-cases\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7224EE-B5FA-490F-874B-03CBA18C18F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E47ED8-319E-4C4F-BE73-7F8864E338F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5BFED0E7-9CB0-4866-AE00-C00A14A216C3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Test Scenario Id</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>System rejects login attempts with invalid credentials</t>
+  </si>
+  <si>
+    <t>RB_TS_06</t>
+  </si>
+  <si>
+    <t>/booking</t>
   </si>
 </sst>
 </file>
@@ -449,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FD3E64-1EED-4B7B-9D72-F3FD21D9A73D}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,6 +533,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added test scenarios for GetBookingIds, GetBooking, CreateBooking
</commit_message>
<xml_diff>
--- a/data/restful_booker_test_scenarios.xlsx
+++ b/data/restful_booker_test_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\restful-booker-test-cases\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E47ED8-319E-4C4F-BE73-7F8864E338F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B067451E-648E-4AEA-9A92-93F6AC70BECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5BFED0E7-9CB0-4866-AE00-C00A14A216C3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5BFED0E7-9CB0-4866-AE00-C00A14A216C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="127">
   <si>
     <t>Test Scenario Id</t>
   </si>
@@ -50,9 +50,6 @@
     <t>RB_TS_01</t>
   </si>
   <si>
-    <t>/auth</t>
-  </si>
-  <si>
     <t>RB_TS_02</t>
   </si>
   <si>
@@ -83,17 +80,359 @@
     <t>RB_TS_06</t>
   </si>
   <si>
-    <t>/booking</t>
+    <t>Filter by first and last names</t>
+  </si>
+  <si>
+    <t>RB_TS_07</t>
+  </si>
+  <si>
+    <t>RB_TS_08</t>
+  </si>
+  <si>
+    <t>RB_TS_09</t>
+  </si>
+  <si>
+    <t>RB_TS_10</t>
+  </si>
+  <si>
+    <t>RB_TS_11</t>
+  </si>
+  <si>
+    <t>RB_TS_12</t>
+  </si>
+  <si>
+    <t>RB_TS_13</t>
+  </si>
+  <si>
+    <t>RB_TS_14</t>
+  </si>
+  <si>
+    <t>RB_TS_15</t>
+  </si>
+  <si>
+    <t>Error for non-existing bookingId</t>
+  </si>
+  <si>
+    <t>Filter by invalid first name</t>
+  </si>
+  <si>
+    <t>Filter by invalid last name</t>
+  </si>
+  <si>
+    <t>Filter by existing first name</t>
+  </si>
+  <si>
+    <t>Filter by existing last name</t>
+  </si>
+  <si>
+    <t>Filter by existing check in date</t>
+  </si>
+  <si>
+    <t>Filter by existing check out date</t>
+  </si>
+  <si>
+    <t>Filter by existing check in and check out dates</t>
+  </si>
+  <si>
+    <t>Filter by existing first name and check in date</t>
+  </si>
+  <si>
+    <t>Filter by existing first name and check out date</t>
+  </si>
+  <si>
+    <t>Filter by existing last name and check in date</t>
+  </si>
+  <si>
+    <t>Filter by existing last name and check out date</t>
+  </si>
+  <si>
+    <t>Filter by check in date with invalid date format</t>
+  </si>
+  <si>
+    <t>Filter by check out date with invalid date format</t>
+  </si>
+  <si>
+    <t>Filter by invalid check in date (string instead of date)</t>
+  </si>
+  <si>
+    <t>Filter by invalid check out date (string instead of date)</t>
+  </si>
+  <si>
+    <t>RB_TS_16</t>
+  </si>
+  <si>
+    <t>RB_TS_17</t>
+  </si>
+  <si>
+    <t>RB_TS_18</t>
+  </si>
+  <si>
+    <t>RB_TS_19</t>
+  </si>
+  <si>
+    <t>RB_TS_20</t>
+  </si>
+  <si>
+    <t>RB_TS_21</t>
+  </si>
+  <si>
+    <t>Read all bookings with no filters</t>
+  </si>
+  <si>
+    <t>RB_TS_22</t>
+  </si>
+  <si>
+    <t>RB_TS_23</t>
+  </si>
+  <si>
+    <t>RB_TS_24</t>
+  </si>
+  <si>
+    <t>POST /auth</t>
+  </si>
+  <si>
+    <t>GET /booking</t>
+  </si>
+  <si>
+    <t>GET /booking/:id</t>
+  </si>
+  <si>
+    <t>POST booking</t>
+  </si>
+  <si>
+    <t>Read existing bookingId (JSON)</t>
+  </si>
+  <si>
+    <t>Read existing bookingId (XML)</t>
+  </si>
+  <si>
+    <t>RB_TS_25</t>
+  </si>
+  <si>
+    <t>Create valid booking (JSON)</t>
+  </si>
+  <si>
+    <t>Create valid booking (XML)</t>
+  </si>
+  <si>
+    <t>Error for booking without first name (JSON)</t>
+  </si>
+  <si>
+    <t>Error for booking without last name (JSON)</t>
+  </si>
+  <si>
+    <t>Error for booking without total price (JSON)</t>
+  </si>
+  <si>
+    <t>Error for booking without deposit paid (JSON)</t>
+  </si>
+  <si>
+    <t>Error for booking without check in date (JSON)</t>
+  </si>
+  <si>
+    <t>Error for booking without check out date (JSON)</t>
+  </si>
+  <si>
+    <t>Error for booking without additional needs (JSON)</t>
+  </si>
+  <si>
+    <t>Error for booking without first name (XML)</t>
+  </si>
+  <si>
+    <t>Error for booking without last name (XML)</t>
+  </si>
+  <si>
+    <t>Error for booking without total price (XML)</t>
+  </si>
+  <si>
+    <t>Error for booking without deposit paid (XML)</t>
+  </si>
+  <si>
+    <t>Error for booking without check in date (XML)</t>
+  </si>
+  <si>
+    <t>Error for booking without check out date (XML)</t>
+  </si>
+  <si>
+    <t>Error for booking without additional needs (XML)</t>
+  </si>
+  <si>
+    <t>RB_TS_26</t>
+  </si>
+  <si>
+    <t>RB_TS_27</t>
+  </si>
+  <si>
+    <t>RB_TS_28</t>
+  </si>
+  <si>
+    <t>RB_TS_29</t>
+  </si>
+  <si>
+    <t>RB_TS_30</t>
+  </si>
+  <si>
+    <t>RB_TS_31</t>
+  </si>
+  <si>
+    <t>RB_TS_32</t>
+  </si>
+  <si>
+    <t>RB_TS_33</t>
+  </si>
+  <si>
+    <t>RB_TS_34</t>
+  </si>
+  <si>
+    <t>RB_TS_35</t>
+  </si>
+  <si>
+    <t>RB_TS_36</t>
+  </si>
+  <si>
+    <t>RB_TS_37</t>
+  </si>
+  <si>
+    <t>RB_TS_38</t>
+  </si>
+  <si>
+    <t>RB_TS_39</t>
+  </si>
+  <si>
+    <t>RB_TS_40</t>
+  </si>
+  <si>
+    <t>RB_TS_41</t>
+  </si>
+  <si>
+    <t>Error for invalid first name (JSON)</t>
+  </si>
+  <si>
+    <t>Error for invalid last name (JSON)</t>
+  </si>
+  <si>
+    <t>Error for invalid total price (negative number) (JSON)</t>
+  </si>
+  <si>
+    <t>Error for invalid deposit paid (JSON)</t>
+  </si>
+  <si>
+    <t>Error for invalid check in date (JSON)</t>
+  </si>
+  <si>
+    <t>Error for invalid check out date (JSON)</t>
+  </si>
+  <si>
+    <t>Error for invalid addtional needs (JSON)</t>
+  </si>
+  <si>
+    <t>Error for invalid first name (XML)</t>
+  </si>
+  <si>
+    <t>Error for invalid last name (XML)</t>
+  </si>
+  <si>
+    <t>Error for invalid total price (negative number) (XML)</t>
+  </si>
+  <si>
+    <t>Error for invalid deposit paid (XML)</t>
+  </si>
+  <si>
+    <t>Error for invalid check in date (XML)</t>
+  </si>
+  <si>
+    <t>Error for invalid check out date (XML)</t>
+  </si>
+  <si>
+    <t>Error for invalid addtional needs (XML)</t>
+  </si>
+  <si>
+    <t>Total price is a decimal (XML)</t>
+  </si>
+  <si>
+    <t>Total price is a decimal (JSON)</t>
+  </si>
+  <si>
+    <t>Error for invalid date format for check in date (JSON)</t>
+  </si>
+  <si>
+    <t>Error for invalid date format check out date (JSON)</t>
+  </si>
+  <si>
+    <t>RB_TS_42</t>
+  </si>
+  <si>
+    <t>RB_TS_43</t>
+  </si>
+  <si>
+    <t>RB_TS_44</t>
+  </si>
+  <si>
+    <t>RB_TS_45</t>
+  </si>
+  <si>
+    <t>RB_TS_46</t>
+  </si>
+  <si>
+    <t>RB_TS_47</t>
+  </si>
+  <si>
+    <t>RB_TS_48</t>
+  </si>
+  <si>
+    <t>RB_TS_49</t>
+  </si>
+  <si>
+    <t>RB_TS_50</t>
+  </si>
+  <si>
+    <t>RB_TS_51</t>
+  </si>
+  <si>
+    <t>RB_TS_52</t>
+  </si>
+  <si>
+    <t>RB_TS_53</t>
+  </si>
+  <si>
+    <t>RB_TS_54</t>
+  </si>
+  <si>
+    <t>RB_TS_55</t>
+  </si>
+  <si>
+    <t>RB_TS_56</t>
+  </si>
+  <si>
+    <t>RB_TS_57</t>
+  </si>
+  <si>
+    <t>RB_TS_58</t>
+  </si>
+  <si>
+    <t>RB_TS_59</t>
+  </si>
+  <si>
+    <t>RB_TS_60</t>
+  </si>
+  <si>
+    <t>RB_TS_61</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -455,16 +794,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FD3E64-1EED-4B7B-9D72-F3FD21D9A73D}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -483,65 +822,674 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" t="s">
+        <v>53</v>
+      </c>
+      <c r="C62" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added prioritization for all test scenarios
</commit_message>
<xml_diff>
--- a/data/restful_booker_test_scenarios.xlsx
+++ b/data/restful_booker_test_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\restful-booker-test-cases\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26D4910-E679-41BF-9B24-19EBE66D1D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0101D32E-40EF-4F4A-8C6C-D7D1864286D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5BFED0E7-9CB0-4866-AE00-C00A14A216C3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5BFED0E7-9CB0-4866-AE00-C00A14A216C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="221">
   <si>
     <t>Test Scenario Id</t>
   </si>
@@ -686,7 +686,19 @@
     <t>Read health check</t>
   </si>
   <si>
-    <t>RB_TS_104</t>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Error for partial update booking with invalid first name (data type other than string) (JSON / XML)</t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FD3E64-1EED-4B7B-9D72-F3FD21D9A73D}">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,6 +1107,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>216</v>
+      </c>
       <c r="C2" t="s">
         <v>49</v>
       </c>
@@ -1106,6 +1121,9 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>216</v>
+      </c>
       <c r="C3" t="s">
         <v>49</v>
       </c>
@@ -1117,6 +1135,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" t="s">
+        <v>216</v>
+      </c>
       <c r="C4" t="s">
         <v>49</v>
       </c>
@@ -1128,6 +1149,9 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="B5" t="s">
+        <v>216</v>
+      </c>
       <c r="C5" t="s">
         <v>49</v>
       </c>
@@ -1139,6 +1163,9 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
+      <c r="B6" t="s">
+        <v>216</v>
+      </c>
       <c r="C6" t="s">
         <v>49</v>
       </c>
@@ -1150,6 +1177,9 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
+      <c r="B7" t="s">
+        <v>217</v>
+      </c>
       <c r="C7" t="s">
         <v>50</v>
       </c>
@@ -1161,6 +1191,9 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
+      <c r="B8" t="s">
+        <v>217</v>
+      </c>
       <c r="C8" t="s">
         <v>50</v>
       </c>
@@ -1172,6 +1205,9 @@
       <c r="A9" t="s">
         <v>16</v>
       </c>
+      <c r="B9" t="s">
+        <v>217</v>
+      </c>
       <c r="C9" t="s">
         <v>50</v>
       </c>
@@ -1183,6 +1219,9 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
+      <c r="B10" t="s">
+        <v>217</v>
+      </c>
       <c r="C10" t="s">
         <v>50</v>
       </c>
@@ -1194,6 +1233,9 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
+      <c r="B11" t="s">
+        <v>217</v>
+      </c>
       <c r="C11" t="s">
         <v>50</v>
       </c>
@@ -1205,6 +1247,9 @@
       <c r="A12" t="s">
         <v>19</v>
       </c>
+      <c r="B12" t="s">
+        <v>217</v>
+      </c>
       <c r="C12" t="s">
         <v>50</v>
       </c>
@@ -1216,6 +1261,9 @@
       <c r="A13" t="s">
         <v>20</v>
       </c>
+      <c r="B13" t="s">
+        <v>217</v>
+      </c>
       <c r="C13" t="s">
         <v>50</v>
       </c>
@@ -1227,6 +1275,9 @@
       <c r="A14" t="s">
         <v>21</v>
       </c>
+      <c r="B14" t="s">
+        <v>217</v>
+      </c>
       <c r="C14" t="s">
         <v>50</v>
       </c>
@@ -1238,6 +1289,9 @@
       <c r="A15" t="s">
         <v>22</v>
       </c>
+      <c r="B15" t="s">
+        <v>217</v>
+      </c>
       <c r="C15" t="s">
         <v>50</v>
       </c>
@@ -1249,6 +1303,9 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
+      <c r="B16" t="s">
+        <v>217</v>
+      </c>
       <c r="C16" t="s">
         <v>50</v>
       </c>
@@ -1260,6 +1317,9 @@
       <c r="A17" t="s">
         <v>39</v>
       </c>
+      <c r="B17" t="s">
+        <v>217</v>
+      </c>
       <c r="C17" t="s">
         <v>50</v>
       </c>
@@ -1271,6 +1331,9 @@
       <c r="A18" t="s">
         <v>40</v>
       </c>
+      <c r="B18" t="s">
+        <v>217</v>
+      </c>
       <c r="C18" t="s">
         <v>50</v>
       </c>
@@ -1282,6 +1345,9 @@
       <c r="A19" t="s">
         <v>41</v>
       </c>
+      <c r="B19" t="s">
+        <v>217</v>
+      </c>
       <c r="C19" t="s">
         <v>50</v>
       </c>
@@ -1293,6 +1359,9 @@
       <c r="A20" t="s">
         <v>42</v>
       </c>
+      <c r="B20" t="s">
+        <v>217</v>
+      </c>
       <c r="C20" t="s">
         <v>50</v>
       </c>
@@ -1304,6 +1373,9 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
+      <c r="B21" t="s">
+        <v>217</v>
+      </c>
       <c r="C21" t="s">
         <v>50</v>
       </c>
@@ -1315,6 +1387,9 @@
       <c r="A22" t="s">
         <v>44</v>
       </c>
+      <c r="B22" t="s">
+        <v>217</v>
+      </c>
       <c r="C22" t="s">
         <v>50</v>
       </c>
@@ -1326,6 +1401,9 @@
       <c r="A23" t="s">
         <v>46</v>
       </c>
+      <c r="B23" t="s">
+        <v>216</v>
+      </c>
       <c r="C23" t="s">
         <v>50</v>
       </c>
@@ -1337,6 +1415,9 @@
       <c r="A24" t="s">
         <v>47</v>
       </c>
+      <c r="B24" t="s">
+        <v>216</v>
+      </c>
       <c r="C24" t="s">
         <v>51</v>
       </c>
@@ -1348,6 +1429,9 @@
       <c r="A25" t="s">
         <v>48</v>
       </c>
+      <c r="B25" t="s">
+        <v>216</v>
+      </c>
       <c r="C25" t="s">
         <v>51</v>
       </c>
@@ -1359,6 +1443,9 @@
       <c r="A26" t="s">
         <v>52</v>
       </c>
+      <c r="B26" t="s">
+        <v>216</v>
+      </c>
       <c r="C26" t="s">
         <v>51</v>
       </c>
@@ -1370,6 +1457,9 @@
       <c r="A27" t="s">
         <v>53</v>
       </c>
+      <c r="B27" t="s">
+        <v>216</v>
+      </c>
       <c r="C27" t="s">
         <v>90</v>
       </c>
@@ -1381,6 +1471,9 @@
       <c r="A28" t="s">
         <v>54</v>
       </c>
+      <c r="B28" t="s">
+        <v>219</v>
+      </c>
       <c r="C28" t="s">
         <v>90</v>
       </c>
@@ -1392,6 +1485,9 @@
       <c r="A29" t="s">
         <v>55</v>
       </c>
+      <c r="B29" t="s">
+        <v>219</v>
+      </c>
       <c r="C29" t="s">
         <v>90</v>
       </c>
@@ -1403,6 +1499,9 @@
       <c r="A30" t="s">
         <v>56</v>
       </c>
+      <c r="B30" t="s">
+        <v>217</v>
+      </c>
       <c r="C30" t="s">
         <v>90</v>
       </c>
@@ -1414,6 +1513,9 @@
       <c r="A31" t="s">
         <v>57</v>
       </c>
+      <c r="B31" t="s">
+        <v>219</v>
+      </c>
       <c r="C31" t="s">
         <v>90</v>
       </c>
@@ -1425,6 +1527,9 @@
       <c r="A32" t="s">
         <v>58</v>
       </c>
+      <c r="B32" t="s">
+        <v>219</v>
+      </c>
       <c r="C32" t="s">
         <v>90</v>
       </c>
@@ -1436,6 +1541,9 @@
       <c r="A33" t="s">
         <v>59</v>
       </c>
+      <c r="B33" t="s">
+        <v>219</v>
+      </c>
       <c r="C33" t="s">
         <v>90</v>
       </c>
@@ -1447,6 +1555,9 @@
       <c r="A34" t="s">
         <v>60</v>
       </c>
+      <c r="B34" t="s">
+        <v>218</v>
+      </c>
       <c r="C34" t="s">
         <v>90</v>
       </c>
@@ -1458,6 +1569,9 @@
       <c r="A35" t="s">
         <v>61</v>
       </c>
+      <c r="B35" t="s">
+        <v>219</v>
+      </c>
       <c r="C35" t="s">
         <v>90</v>
       </c>
@@ -1469,6 +1583,9 @@
       <c r="A36" t="s">
         <v>62</v>
       </c>
+      <c r="B36" t="s">
+        <v>219</v>
+      </c>
       <c r="C36" t="s">
         <v>90</v>
       </c>
@@ -1480,6 +1597,9 @@
       <c r="A37" t="s">
         <v>63</v>
       </c>
+      <c r="B37" t="s">
+        <v>217</v>
+      </c>
       <c r="C37" t="s">
         <v>90</v>
       </c>
@@ -1491,6 +1611,9 @@
       <c r="A38" t="s">
         <v>64</v>
       </c>
+      <c r="B38" t="s">
+        <v>217</v>
+      </c>
       <c r="C38" t="s">
         <v>90</v>
       </c>
@@ -1502,6 +1625,9 @@
       <c r="A39" t="s">
         <v>65</v>
       </c>
+      <c r="B39" t="s">
+        <v>219</v>
+      </c>
       <c r="C39" t="s">
         <v>90</v>
       </c>
@@ -1513,6 +1639,9 @@
       <c r="A40" t="s">
         <v>66</v>
       </c>
+      <c r="B40" t="s">
+        <v>219</v>
+      </c>
       <c r="C40" t="s">
         <v>90</v>
       </c>
@@ -1524,6 +1653,9 @@
       <c r="A41" t="s">
         <v>67</v>
       </c>
+      <c r="B41" t="s">
+        <v>218</v>
+      </c>
       <c r="C41" t="s">
         <v>90</v>
       </c>
@@ -1535,6 +1667,9 @@
       <c r="A42" t="s">
         <v>68</v>
       </c>
+      <c r="B42" t="s">
+        <v>219</v>
+      </c>
       <c r="C42" t="s">
         <v>90</v>
       </c>
@@ -1546,6 +1681,9 @@
       <c r="A43" t="s">
         <v>69</v>
       </c>
+      <c r="B43" t="s">
+        <v>219</v>
+      </c>
       <c r="C43" t="s">
         <v>90</v>
       </c>
@@ -1557,6 +1695,9 @@
       <c r="A44" t="s">
         <v>70</v>
       </c>
+      <c r="B44" t="s">
+        <v>219</v>
+      </c>
       <c r="C44" t="s">
         <v>90</v>
       </c>
@@ -1568,6 +1709,9 @@
       <c r="A45" t="s">
         <v>71</v>
       </c>
+      <c r="B45" t="s">
+        <v>216</v>
+      </c>
       <c r="C45" t="s">
         <v>204</v>
       </c>
@@ -1579,6 +1723,9 @@
       <c r="A46" t="s">
         <v>72</v>
       </c>
+      <c r="B46" t="s">
+        <v>216</v>
+      </c>
       <c r="C46" t="s">
         <v>204</v>
       </c>
@@ -1590,6 +1737,9 @@
       <c r="A47" t="s">
         <v>73</v>
       </c>
+      <c r="B47" t="s">
+        <v>216</v>
+      </c>
       <c r="C47" t="s">
         <v>204</v>
       </c>
@@ -1601,6 +1751,9 @@
       <c r="A48" t="s">
         <v>74</v>
       </c>
+      <c r="B48" t="s">
+        <v>216</v>
+      </c>
       <c r="C48" t="s">
         <v>204</v>
       </c>
@@ -1612,6 +1765,9 @@
       <c r="A49" t="s">
         <v>75</v>
       </c>
+      <c r="B49" t="s">
+        <v>216</v>
+      </c>
       <c r="C49" t="s">
         <v>204</v>
       </c>
@@ -1623,6 +1779,9 @@
       <c r="A50" t="s">
         <v>76</v>
       </c>
+      <c r="B50" t="s">
+        <v>216</v>
+      </c>
       <c r="C50" t="s">
         <v>204</v>
       </c>
@@ -1634,6 +1793,9 @@
       <c r="A51" t="s">
         <v>77</v>
       </c>
+      <c r="B51" t="s">
+        <v>217</v>
+      </c>
       <c r="C51" t="s">
         <v>204</v>
       </c>
@@ -1645,6 +1807,9 @@
       <c r="A52" t="s">
         <v>78</v>
       </c>
+      <c r="B52" t="s">
+        <v>217</v>
+      </c>
       <c r="C52" t="s">
         <v>204</v>
       </c>
@@ -1656,6 +1821,9 @@
       <c r="A53" t="s">
         <v>79</v>
       </c>
+      <c r="B53" t="s">
+        <v>217</v>
+      </c>
       <c r="C53" t="s">
         <v>204</v>
       </c>
@@ -1667,6 +1835,9 @@
       <c r="A54" t="s">
         <v>80</v>
       </c>
+      <c r="B54" t="s">
+        <v>217</v>
+      </c>
       <c r="C54" t="s">
         <v>204</v>
       </c>
@@ -1678,6 +1849,9 @@
       <c r="A55" t="s">
         <v>81</v>
       </c>
+      <c r="B55" t="s">
+        <v>217</v>
+      </c>
       <c r="C55" t="s">
         <v>204</v>
       </c>
@@ -1689,6 +1863,9 @@
       <c r="A56" t="s">
         <v>82</v>
       </c>
+      <c r="B56" t="s">
+        <v>219</v>
+      </c>
       <c r="C56" t="s">
         <v>204</v>
       </c>
@@ -1700,6 +1877,9 @@
       <c r="A57" t="s">
         <v>83</v>
       </c>
+      <c r="B57" t="s">
+        <v>219</v>
+      </c>
       <c r="C57" t="s">
         <v>204</v>
       </c>
@@ -1711,6 +1891,9 @@
       <c r="A58" t="s">
         <v>84</v>
       </c>
+      <c r="B58" t="s">
+        <v>218</v>
+      </c>
       <c r="C58" t="s">
         <v>204</v>
       </c>
@@ -1722,6 +1905,9 @@
       <c r="A59" t="s">
         <v>85</v>
       </c>
+      <c r="B59" t="s">
+        <v>217</v>
+      </c>
       <c r="C59" t="s">
         <v>204</v>
       </c>
@@ -1733,6 +1919,9 @@
       <c r="A60" t="s">
         <v>86</v>
       </c>
+      <c r="B60" t="s">
+        <v>217</v>
+      </c>
       <c r="C60" t="s">
         <v>204</v>
       </c>
@@ -1744,6 +1933,9 @@
       <c r="A61" t="s">
         <v>87</v>
       </c>
+      <c r="B61" t="s">
+        <v>217</v>
+      </c>
       <c r="C61" t="s">
         <v>204</v>
       </c>
@@ -1755,6 +1947,9 @@
       <c r="A62" t="s">
         <v>88</v>
       </c>
+      <c r="B62" t="s">
+        <v>217</v>
+      </c>
       <c r="C62" t="s">
         <v>204</v>
       </c>
@@ -1766,6 +1961,9 @@
       <c r="A63" t="s">
         <v>135</v>
       </c>
+      <c r="B63" t="s">
+        <v>219</v>
+      </c>
       <c r="C63" t="s">
         <v>204</v>
       </c>
@@ -1777,6 +1975,9 @@
       <c r="A64" t="s">
         <v>136</v>
       </c>
+      <c r="B64" t="s">
+        <v>219</v>
+      </c>
       <c r="C64" t="s">
         <v>204</v>
       </c>
@@ -1788,6 +1989,9 @@
       <c r="A65" t="s">
         <v>137</v>
       </c>
+      <c r="B65" t="s">
+        <v>218</v>
+      </c>
       <c r="C65" t="s">
         <v>204</v>
       </c>
@@ -1799,6 +2003,9 @@
       <c r="A66" t="s">
         <v>138</v>
       </c>
+      <c r="B66" t="s">
+        <v>219</v>
+      </c>
       <c r="C66" t="s">
         <v>204</v>
       </c>
@@ -1810,6 +2017,9 @@
       <c r="A67" t="s">
         <v>139</v>
       </c>
+      <c r="B67" t="s">
+        <v>219</v>
+      </c>
       <c r="C67" t="s">
         <v>204</v>
       </c>
@@ -1821,6 +2031,9 @@
       <c r="A68" t="s">
         <v>147</v>
       </c>
+      <c r="B68" t="s">
+        <v>217</v>
+      </c>
       <c r="C68" t="s">
         <v>204</v>
       </c>
@@ -1832,411 +2045,509 @@
       <c r="A69" t="s">
         <v>148</v>
       </c>
+      <c r="B69" t="s">
+        <v>219</v>
+      </c>
       <c r="C69" t="s">
         <v>204</v>
       </c>
       <c r="D69" t="s">
-        <v>116</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>149</v>
       </c>
+      <c r="B70" t="s">
+        <v>216</v>
+      </c>
       <c r="C70" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D70" t="s">
-        <v>207</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>150</v>
       </c>
+      <c r="B71" t="s">
+        <v>216</v>
+      </c>
       <c r="C71" t="s">
         <v>205</v>
       </c>
       <c r="D71" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>151</v>
       </c>
+      <c r="B72" t="s">
+        <v>216</v>
+      </c>
       <c r="C72" t="s">
         <v>205</v>
       </c>
       <c r="D72" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>152</v>
       </c>
+      <c r="B73" t="s">
+        <v>216</v>
+      </c>
       <c r="C73" t="s">
         <v>205</v>
       </c>
       <c r="D73" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>153</v>
       </c>
+      <c r="B74" t="s">
+        <v>216</v>
+      </c>
       <c r="C74" t="s">
         <v>205</v>
       </c>
       <c r="D74" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>170</v>
       </c>
+      <c r="B75" t="s">
+        <v>216</v>
+      </c>
       <c r="C75" t="s">
         <v>205</v>
       </c>
       <c r="D75" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>171</v>
       </c>
+      <c r="B76" t="s">
+        <v>217</v>
+      </c>
       <c r="C76" t="s">
         <v>205</v>
       </c>
       <c r="D76" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>172</v>
       </c>
+      <c r="B77" t="s">
+        <v>219</v>
+      </c>
       <c r="C77" t="s">
         <v>205</v>
       </c>
       <c r="D77" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>173</v>
       </c>
+      <c r="B78" t="s">
+        <v>219</v>
+      </c>
       <c r="C78" t="s">
         <v>205</v>
       </c>
       <c r="D78" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>174</v>
       </c>
+      <c r="B79" t="s">
+        <v>219</v>
+      </c>
       <c r="C79" t="s">
         <v>205</v>
       </c>
       <c r="D79" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>175</v>
       </c>
+      <c r="B80" t="s">
+        <v>219</v>
+      </c>
       <c r="C80" t="s">
         <v>205</v>
       </c>
       <c r="D80" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>176</v>
       </c>
+      <c r="B81" t="s">
+        <v>219</v>
+      </c>
       <c r="C81" t="s">
         <v>205</v>
       </c>
       <c r="D81" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>177</v>
       </c>
+      <c r="B82" t="s">
+        <v>219</v>
+      </c>
       <c r="C82" t="s">
         <v>205</v>
       </c>
       <c r="D82" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>178</v>
       </c>
+      <c r="B83" t="s">
+        <v>218</v>
+      </c>
       <c r="C83" t="s">
         <v>205</v>
       </c>
       <c r="D83" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>179</v>
       </c>
+      <c r="B84" t="s">
+        <v>217</v>
+      </c>
       <c r="C84" t="s">
         <v>205</v>
       </c>
       <c r="D84" t="s">
-        <v>160</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>180</v>
       </c>
+      <c r="B85" t="s">
+        <v>217</v>
+      </c>
       <c r="C85" t="s">
         <v>205</v>
       </c>
       <c r="D85" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>181</v>
       </c>
+      <c r="B86" t="s">
+        <v>217</v>
+      </c>
       <c r="C86" t="s">
         <v>205</v>
       </c>
       <c r="D86" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>182</v>
       </c>
+      <c r="B87" t="s">
+        <v>217</v>
+      </c>
       <c r="C87" t="s">
         <v>205</v>
       </c>
       <c r="D87" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>183</v>
       </c>
+      <c r="B88" t="s">
+        <v>219</v>
+      </c>
       <c r="C88" t="s">
         <v>205</v>
       </c>
       <c r="D88" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>184</v>
       </c>
+      <c r="B89" t="s">
+        <v>219</v>
+      </c>
       <c r="C89" t="s">
         <v>205</v>
       </c>
       <c r="D89" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>185</v>
       </c>
+      <c r="B90" t="s">
+        <v>218</v>
+      </c>
       <c r="C90" t="s">
         <v>205</v>
       </c>
       <c r="D90" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>186</v>
       </c>
+      <c r="B91" t="s">
+        <v>219</v>
+      </c>
       <c r="C91" t="s">
         <v>205</v>
       </c>
       <c r="D91" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>194</v>
       </c>
+      <c r="B92" t="s">
+        <v>219</v>
+      </c>
       <c r="C92" t="s">
         <v>205</v>
       </c>
       <c r="D92" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>195</v>
       </c>
+      <c r="B93" t="s">
+        <v>217</v>
+      </c>
       <c r="C93" t="s">
         <v>205</v>
       </c>
       <c r="D93" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>196</v>
       </c>
+      <c r="B94" t="s">
+        <v>219</v>
+      </c>
       <c r="C94" t="s">
         <v>205</v>
       </c>
       <c r="D94" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>197</v>
       </c>
+      <c r="B95" t="s">
+        <v>219</v>
+      </c>
       <c r="C95" t="s">
         <v>205</v>
       </c>
       <c r="D95" t="s">
-        <v>146</v>
+        <v>208</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>198</v>
       </c>
+      <c r="B96" t="s">
+        <v>216</v>
+      </c>
       <c r="C96" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D96" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>199</v>
       </c>
+      <c r="B97" t="s">
+        <v>216</v>
+      </c>
       <c r="C97" t="s">
         <v>206</v>
       </c>
       <c r="D97" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>200</v>
       </c>
+      <c r="B98" t="s">
+        <v>216</v>
+      </c>
       <c r="C98" t="s">
         <v>206</v>
       </c>
       <c r="D98" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>203</v>
       </c>
+      <c r="B99" t="s">
+        <v>216</v>
+      </c>
       <c r="C99" t="s">
         <v>206</v>
       </c>
       <c r="D99" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>209</v>
       </c>
+      <c r="B100" t="s">
+        <v>216</v>
+      </c>
       <c r="C100" t="s">
         <v>206</v>
       </c>
       <c r="D100" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>210</v>
       </c>
+      <c r="B101" t="s">
+        <v>216</v>
+      </c>
       <c r="C101" t="s">
         <v>206</v>
       </c>
       <c r="D101" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>211</v>
       </c>
+      <c r="B102" t="s">
+        <v>216</v>
+      </c>
       <c r="C102" t="s">
         <v>206</v>
       </c>
       <c r="D102" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>212</v>
       </c>
+      <c r="B103" t="s">
+        <v>216</v>
+      </c>
       <c r="C103" t="s">
         <v>206</v>
       </c>
       <c r="D103" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>213</v>
       </c>
+      <c r="B104" t="s">
+        <v>216</v>
+      </c>
       <c r="C104" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="D104" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>216</v>
-      </c>
-      <c r="C105" t="s">
-        <v>214</v>
-      </c>
-      <c r="D105" t="s">
         <v>215</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>